<commit_message>
Moved VA from LOSO to LONE
</commit_message>
<xml_diff>
--- a/TaxableGallons_gas.xlsx
+++ b/TaxableGallons_gas.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021\OPIS\Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E461A88A-96C3-4B6A-BAF9-5504F12309D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A457BF6C-4705-4F4A-BDE3-B90207172B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="2910" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gallons_Change" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gallons_Change!$A$1:$H$50</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
   <si>
     <t>State</t>
   </si>
@@ -349,6 +353,12 @@
   </si>
   <si>
     <t>Northeast</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
@@ -491,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +679,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -832,12 +848,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1193,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,33 +1221,33 @@
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="5">
         <v>2021</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="5">
         <v>2020</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="5">
         <v>2019</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1253,10 +1270,10 @@
       <c r="F2" s="3">
         <v>657608737</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>1.44E-2</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>0.14469145047262352</v>
       </c>
     </row>
@@ -1276,10 +1293,10 @@
       <c r="F3" s="3">
         <v>737248299</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>-5.0500000000000003E-2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>-4.2513701343921309E-2</v>
       </c>
     </row>
@@ -1302,10 +1319,10 @@
       <c r="F4" s="3">
         <v>361032694</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>-2.9399999999999999E-2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>-3.5789761466865931E-2</v>
       </c>
     </row>
@@ -1325,10 +1342,10 @@
       <c r="F5" s="3">
         <v>3673655242</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>-9.6000000000000002E-2</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>-0.15323304173026697</v>
       </c>
     </row>
@@ -1348,10 +1365,10 @@
       <c r="F6" s="3">
         <v>571763985</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>-3.5900000000000001E-2</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="2">
         <v>-9.0457705201561447E-2</v>
       </c>
     </row>
@@ -1374,10 +1391,10 @@
       <c r="F7" s="3">
         <v>359235840</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>-0.15659999999999999</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>-0.20235007175230624</v>
       </c>
     </row>
@@ -1400,10 +1417,10 @@
       <c r="F8" s="3">
         <v>126363854</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>-0.1328</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>-0.14435587727484159</v>
       </c>
     </row>
@@ -1423,10 +1440,10 @@
       <c r="F9" s="3">
         <v>29603981</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>-8.5400000000000004E-2</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>-0.13443806763691679</v>
       </c>
     </row>
@@ -1449,10 +1466,10 @@
       <c r="F10" s="3">
         <v>2298537833</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>-9.1999999999999998E-2</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>-7.5151372546496606E-2</v>
       </c>
     </row>
@@ -1475,10 +1492,10 @@
       <c r="F11" s="3">
         <v>1202455590</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>3.1773023733874446E-3</v>
       </c>
     </row>
@@ -1498,10 +1515,10 @@
       <c r="F12" s="3">
         <v>193483015</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>4.7800000000000002E-2</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>2.7987603976504089E-2</v>
       </c>
     </row>
@@ -1524,10 +1541,10 @@
       <c r="F13" s="3">
         <v>1161591306</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>-7.9100000000000004E-2</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>-0.16809331732377825</v>
       </c>
     </row>
@@ -1550,10 +1567,10 @@
       <c r="F14" s="3">
         <v>734036173</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>-1.37E-2</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>-3.1546299558182674E-2</v>
       </c>
     </row>
@@ -1573,10 +1590,10 @@
       <c r="F15" s="3">
         <v>379545398</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>-2.18E-2</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>-4.1195638472739431E-2</v>
       </c>
     </row>
@@ -1596,10 +1613,10 @@
       <c r="F16" s="3">
         <v>283268621</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <v>-2.8799999999999999E-2</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="2">
         <v>1.8539907390589513E-2</v>
       </c>
     </row>
@@ -1622,10 +1639,10 @@
       <c r="F17" s="3">
         <v>526152421</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <v>-5.6599999999999998E-2</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="2">
         <v>-7.2224939928576329E-2</v>
       </c>
     </row>
@@ -1648,10 +1665,10 @@
       <c r="F18" s="3">
         <v>557218346</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>-0.1037</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>-0.16166507195367899</v>
       </c>
     </row>
@@ -1674,10 +1691,10 @@
       <c r="F19" s="3">
         <v>216278953</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>-0.1817</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="2">
         <v>-0.3487339195691409</v>
       </c>
     </row>
@@ -1700,10 +1717,10 @@
       <c r="F20" s="3">
         <v>645990859</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>5.9799999999999999E-2</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>-9.9053348988642584E-2</v>
       </c>
     </row>
@@ -1726,10 +1743,10 @@
       <c r="F21" s="3">
         <v>663008277</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <v>-0.16569999999999999</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="2">
         <v>-0.22486801322391334</v>
       </c>
     </row>
@@ -1752,10 +1769,10 @@
       <c r="F22" s="3">
         <v>1117291516</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <v>-0.1231</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="2">
         <v>-0.16302806330447425</v>
       </c>
     </row>
@@ -1775,10 +1792,10 @@
       <c r="F23" s="3">
         <v>623976374</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2">
         <v>-0.1394</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="2">
         <v>-0.12961659186153737</v>
       </c>
     </row>
@@ -1801,10 +1818,10 @@
       <c r="F24" s="3">
         <v>395807980</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2">
         <v>-9.9699999999999997E-2</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="2">
         <v>-7.1480365302387286E-2</v>
       </c>
     </row>
@@ -1824,10 +1841,10 @@
       <c r="F25" s="3">
         <v>734064029</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2">
         <v>-0.10199999999999999</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="2">
         <v>-4.6597832952798179E-2</v>
       </c>
     </row>
@@ -1847,10 +1864,10 @@
       <c r="F26" s="3">
         <v>118596344</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="2">
         <v>7.3300000000000004E-2</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="2">
         <v>4.0739763444984443E-2</v>
       </c>
     </row>
@@ -1870,10 +1887,10 @@
       <c r="F27" s="3">
         <v>209469224</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2">
         <v>-6.6000000000000003E-2</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="2">
         <v>-6.2261824200007539E-2</v>
       </c>
     </row>
@@ -1893,10 +1910,10 @@
       <c r="F28" s="3">
         <v>293025053</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2">
         <v>-3.9300000000000002E-2</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="2">
         <v>-7.5902571375014813E-2</v>
       </c>
     </row>
@@ -1919,10 +1936,10 @@
       <c r="F29" s="3">
         <v>174709417</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="2">
         <v>-0.1268</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="2">
         <v>-0.17592289830604838</v>
       </c>
     </row>
@@ -1945,10 +1962,10 @@
       <c r="F30" s="3">
         <v>940879482</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2">
         <v>-9.5600000000000004E-2</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="2">
         <v>-0.18618871104259024</v>
       </c>
     </row>
@@ -1968,10 +1985,10 @@
       <c r="F31" s="3">
         <v>249255137</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="2">
         <v>-5.3E-3</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="2">
         <v>-2.6643976448918683E-2</v>
       </c>
     </row>
@@ -1994,10 +2011,10 @@
       <c r="F32" s="3">
         <v>1447864591</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2">
         <v>-0.1484</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="2">
         <v>-0.24016194964740317</v>
       </c>
     </row>
@@ -2020,10 +2037,10 @@
       <c r="F33" s="3">
         <v>1197881836</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="2">
         <v>-7.5800000000000006E-2</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="2">
         <v>-0.13801633936788402</v>
       </c>
     </row>
@@ -2043,10 +2060,10 @@
       <c r="F34" s="3">
         <v>100281591</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2">
         <v>-1.4200000000000001E-2</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="2">
         <v>-1.8151786203711107E-2</v>
       </c>
     </row>
@@ -2066,10 +2083,10 @@
       <c r="F35" s="3">
         <v>1194214252</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="2">
         <v>-6.0900000000000003E-2</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="2">
         <v>-9.400514925356962E-2</v>
       </c>
     </row>
@@ -2089,10 +2106,10 @@
       <c r="F36" s="3">
         <v>435402759</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="2">
         <v>-7.4399999999999994E-2</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="2">
         <v>9.3166382530892504E-4</v>
       </c>
     </row>
@@ -2112,10 +2129,10 @@
       <c r="F37" s="3">
         <v>370073394</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="2">
         <v>-4.7800000000000002E-2</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="2">
         <v>-8.2998028223558271E-2</v>
       </c>
     </row>
@@ -2138,10 +2155,10 @@
       <c r="F38" s="3">
         <v>1154663171</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="2">
         <v>-8.8599999999999998E-2</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38" s="2">
         <v>-0.11310555084812694</v>
       </c>
     </row>
@@ -2164,10 +2181,10 @@
       <c r="F39" s="3">
         <v>93420908</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2">
         <v>-6.0100000000000001E-2</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="2">
         <v>-0.12637218212436985</v>
       </c>
     </row>
@@ -2190,10 +2207,10 @@
       <c r="F40" s="3">
         <v>686688466</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2">
         <v>5.4600000000000003E-2</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="2">
         <v>-2.7263521854464932E-2</v>
       </c>
     </row>
@@ -2213,10 +2230,10 @@
       <c r="F41" s="3">
         <v>103624715</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2">
         <v>-0.03</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="2">
         <v>1.2986477212506687E-2</v>
       </c>
     </row>
@@ -2239,10 +2256,10 @@
       <c r="F42" s="3">
         <v>799773225</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="2">
         <v>-7.8100000000000003E-2</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="2">
         <v>-7.1804936955722667E-2</v>
       </c>
     </row>
@@ -2265,10 +2282,10 @@
       <c r="F43" s="3">
         <v>3603722641</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="2">
         <v>-6.7199999999999996E-2</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="2">
         <v>-9.9636004701062125E-2</v>
       </c>
     </row>
@@ -2288,10 +2305,10 @@
       <c r="F44" s="3">
         <v>293402562</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="2">
         <v>-7.7200000000000005E-2</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="2">
         <v>-7.6920476924806136E-2</v>
       </c>
     </row>
@@ -2314,10 +2331,10 @@
       <c r="F45" s="3">
         <v>74565756</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="2">
         <v>-0.13789999999999999</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="2">
         <v>-0.20974500680982835</v>
       </c>
     </row>
@@ -2328,8 +2345,8 @@
       <c r="B46" t="s">
         <v>94</v>
       </c>
-      <c r="C46" t="s">
-        <v>103</v>
+      <c r="C46" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="D46" s="3">
         <v>835786237</v>
@@ -2340,10 +2357,10 @@
       <c r="F46" s="3">
         <v>1065760080</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="2">
         <v>-6.4399999999999999E-2</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="2">
         <v>-0.21578387792494536</v>
       </c>
     </row>
@@ -2363,10 +2380,10 @@
       <c r="F47" s="3">
         <v>651756456</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="2">
         <v>-7.5899999999999995E-2</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="2">
         <v>-0.11625034980857941</v>
       </c>
     </row>
@@ -2389,10 +2406,10 @@
       <c r="F48" s="3">
         <v>187702979</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="2">
         <v>-1.6899999999999998E-2</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48" s="2">
         <v>-4.2405555001873464E-2</v>
       </c>
     </row>
@@ -2415,10 +2432,10 @@
       <c r="F49" s="3">
         <v>618201893</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2">
         <v>-8.8200000000000001E-2</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49" s="2">
         <v>-0.10326275238371035</v>
       </c>
     </row>
@@ -2438,27 +2455,426 @@
       <c r="F50" s="3">
         <v>77844507</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="2">
         <v>-4.7199999999999999E-2</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50" s="2">
         <v>-4.7792517974325405E-2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G51" s="4">
-        <f>SUM(G2:G50)</f>
-        <v>-3.1240000000000006</v>
-      </c>
-      <c r="H51" s="4">
-        <f>SUM(H2:H50)</f>
-        <v>-4.5379348000776414</v>
-      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C52">
     <sortCondition ref="A2:A52"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4CF1EF-58BD-4E08-B072-F98F861F020E}">
+  <dimension ref="A1:I54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="3">
+        <v>752759099</v>
+      </c>
+      <c r="E1" s="3">
+        <v>742036919</v>
+      </c>
+      <c r="F1" s="3">
+        <v>657608737</v>
+      </c>
+      <c r="G1" s="2">
+        <v>1.44E-2</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0.14469145047262352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2125799560</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2341276306</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2298537833</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-7.5151372546496606E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1206276155</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1198886410</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1202455590</v>
+      </c>
+      <c r="G3" s="2">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3.1773023733874446E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="3">
+        <v>488151094</v>
+      </c>
+      <c r="E4" s="3">
+        <v>517456079</v>
+      </c>
+      <c r="F4" s="3">
+        <v>526152421</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-5.6599999999999998E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>-7.2224939928576329E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="3">
+        <v>367515481</v>
+      </c>
+      <c r="E5" s="3">
+        <v>408230744</v>
+      </c>
+      <c r="F5" s="3">
+        <v>395807980</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-9.9699999999999997E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-7.1480365302387286E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1032554570</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1117254237</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1197881836</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-7.5800000000000006E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>-0.13801633936788402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="3">
+        <v>667966920</v>
+      </c>
+      <c r="E7" s="3">
+        <v>633402028</v>
+      </c>
+      <c r="F7" s="3">
+        <v>686688466</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-2.7263521854464932E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="3">
+        <v>742345559</v>
+      </c>
+      <c r="E8" s="3">
+        <v>805277619</v>
+      </c>
+      <c r="F8" s="3">
+        <v>799773225</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-7.8100000000000003E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-7.1804936955722667E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="3">
+        <v>835786237</v>
+      </c>
+      <c r="E9" s="3">
+        <v>893357769</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1065760080</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-6.4399999999999999E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>-0.21578387792494536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D52" s="1"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" s="3">
+        <f>MIN(D2:D50)</f>
+        <v>367515481</v>
+      </c>
+      <c r="F53" s="3">
+        <f>MIN(E2:E50)</f>
+        <v>408230744</v>
+      </c>
+      <c r="G53" s="3">
+        <f>MIN(F2:F50)</f>
+        <v>395807980</v>
+      </c>
+      <c r="H53" s="4">
+        <f>MIN(G2:G50)</f>
+        <v>-9.9699999999999997E-2</v>
+      </c>
+      <c r="I53" s="4">
+        <f>MIN(H2:H50)</f>
+        <v>-0.21578387792494536</v>
+      </c>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="3">
+        <f>MAX(D2:D50)</f>
+        <v>2125799560</v>
+      </c>
+      <c r="F54" s="3">
+        <f>MAX(E2:E50)</f>
+        <v>2341276306</v>
+      </c>
+      <c r="G54" s="3">
+        <f>MAX(F2:F50)</f>
+        <v>2298537833</v>
+      </c>
+      <c r="H54" s="4">
+        <f>MAX(G2:G50)</f>
+        <v>5.4600000000000003E-2</v>
+      </c>
+      <c r="I54" s="4">
+        <f>MAX(H2:H50)</f>
+        <v>3.1773023733874446E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved VA back to LOSO
</commit_message>
<xml_diff>
--- a/TaxableGallons_gas.xlsx
+++ b/TaxableGallons_gas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\2021\OPIS\Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A457BF6C-4705-4F4A-BDE3-B90207172B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FCDFF5-0F6C-45D4-A9FB-FFD81914D27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1213,7 +1213,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,7 +2346,7 @@
         <v>94</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D46" s="3">
         <v>835786237</v>

</xml_diff>